<commit_message>
Cambios en archivo Clientes
</commit_message>
<xml_diff>
--- a/ClientesDatos.xlsx
+++ b/ClientesDatos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Lenguaje De Programación 2018-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\MyBanco\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="252">
   <si>
     <t>F</t>
   </si>
@@ -650,6 +650,159 @@
   </si>
   <si>
     <t>eguti@hotmail.com</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>sc4535</t>
+  </si>
+  <si>
+    <t>as9874</t>
+  </si>
+  <si>
+    <t>jg9694</t>
+  </si>
+  <si>
+    <t>ac5982</t>
+  </si>
+  <si>
+    <t>at6460</t>
+  </si>
+  <si>
+    <t>av7311</t>
+  </si>
+  <si>
+    <t>ac6387</t>
+  </si>
+  <si>
+    <t>ac7704</t>
+  </si>
+  <si>
+    <t>ab6500</t>
+  </si>
+  <si>
+    <t>bb4484</t>
+  </si>
+  <si>
+    <t>cg7798</t>
+  </si>
+  <si>
+    <t>cg3402</t>
+  </si>
+  <si>
+    <t>cm7210</t>
+  </si>
+  <si>
+    <t>df6624</t>
+  </si>
+  <si>
+    <t>dm8518</t>
+  </si>
+  <si>
+    <t>er8719</t>
+  </si>
+  <si>
+    <t>gr7529</t>
+  </si>
+  <si>
+    <t>hb1423</t>
+  </si>
+  <si>
+    <t>hb2334</t>
+  </si>
+  <si>
+    <t>jc1521</t>
+  </si>
+  <si>
+    <t>jg7972</t>
+  </si>
+  <si>
+    <t>jg2849</t>
+  </si>
+  <si>
+    <t>jm6926</t>
+  </si>
+  <si>
+    <t>jm1039</t>
+  </si>
+  <si>
+    <t>jp1588</t>
+  </si>
+  <si>
+    <t>la1846</t>
+  </si>
+  <si>
+    <t>mt7379</t>
+  </si>
+  <si>
+    <t>pp1660</t>
+  </si>
+  <si>
+    <t>sv6778</t>
+  </si>
+  <si>
+    <t>vp3544</t>
+  </si>
+  <si>
+    <t>vg1340</t>
+  </si>
+  <si>
+    <t>lg3416</t>
+  </si>
+  <si>
+    <t>jb2618</t>
+  </si>
+  <si>
+    <t>bg4412</t>
+  </si>
+  <si>
+    <t>ks7804</t>
+  </si>
+  <si>
+    <t>md5980</t>
+  </si>
+  <si>
+    <t>dn8579</t>
+  </si>
+  <si>
+    <t>ab6130</t>
+  </si>
+  <si>
+    <t>jl3163</t>
+  </si>
+  <si>
+    <t>ca8995</t>
+  </si>
+  <si>
+    <t>ec1392</t>
+  </si>
+  <si>
+    <t>av9265</t>
+  </si>
+  <si>
+    <t>ap1167</t>
+  </si>
+  <si>
+    <t>bg4146</t>
+  </si>
+  <si>
+    <t>ac5143</t>
+  </si>
+  <si>
+    <t>af2778</t>
+  </si>
+  <si>
+    <t>ms817440</t>
+  </si>
+  <si>
+    <t>ej3374</t>
+  </si>
+  <si>
+    <t>gc4936</t>
+  </si>
+  <si>
+    <t>eg6092</t>
   </si>
 </sst>
 </file>
@@ -719,7 +872,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -742,12 +895,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -778,6 +942,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1060,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="I2" sqref="I2:I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,9 +1245,10 @@
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" customWidth="1"/>
     <col min="8" max="8" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
@@ -1102,8 +1273,11 @@
       <c r="H1" s="9" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="13" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1128,8 +1302,11 @@
       <c r="H2" s="11">
         <v>36146</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1154,8 +1331,11 @@
       <c r="H3" s="10">
         <v>36778</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
@@ -1180,8 +1360,11 @@
       <c r="H4" s="10">
         <v>33649</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -1206,8 +1389,11 @@
       <c r="H5" s="10">
         <v>32516</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
@@ -1232,8 +1418,11 @@
       <c r="H6" s="10">
         <v>36257</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="14" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -1258,8 +1447,11 @@
       <c r="H7" s="10">
         <v>30008</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="14" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
@@ -1284,8 +1476,11 @@
       <c r="H8" s="10">
         <v>33379</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
@@ -1310,8 +1505,11 @@
       <c r="H9" s="10">
         <v>36200</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="14" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -1336,8 +1534,11 @@
       <c r="H10" s="10">
         <v>31978</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="14" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
@@ -1362,8 +1563,11 @@
       <c r="H11" s="10">
         <v>31410</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
@@ -1388,8 +1592,11 @@
       <c r="H12" s="10">
         <v>33491</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="14" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>35</v>
       </c>
@@ -1414,8 +1621,11 @@
       <c r="H13" s="10">
         <v>36050</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>37</v>
       </c>
@@ -1440,8 +1650,11 @@
       <c r="H14" s="10">
         <v>35275</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>39</v>
       </c>
@@ -1466,8 +1679,11 @@
       <c r="H15" s="10">
         <v>30938</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>41</v>
       </c>
@@ -1492,8 +1708,11 @@
       <c r="H16" s="10">
         <v>33081</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="14" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>43</v>
       </c>
@@ -1518,8 +1737,11 @@
       <c r="H17" s="10">
         <v>31877</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="14" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>45</v>
       </c>
@@ -1544,8 +1766,11 @@
       <c r="H18" s="10">
         <v>34638</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>47</v>
       </c>
@@ -1570,8 +1795,11 @@
       <c r="H19" s="10">
         <v>34645</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="14" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>49</v>
       </c>
@@ -1596,8 +1824,11 @@
       <c r="H20" s="10">
         <v>34735</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="14" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>51</v>
       </c>
@@ -1622,8 +1853,11 @@
       <c r="H21" s="10">
         <v>34288</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>53</v>
       </c>
@@ -1648,8 +1882,11 @@
       <c r="H22" s="10">
         <v>36474</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="14" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>18</v>
       </c>
@@ -1674,8 +1911,11 @@
       <c r="H23" s="10">
         <v>33521</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="14" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>18</v>
       </c>
@@ -1700,8 +1940,11 @@
       <c r="H24" s="10">
         <v>33550</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>57</v>
       </c>
@@ -1726,8 +1969,11 @@
       <c r="H25" s="10">
         <v>33732</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>59</v>
       </c>
@@ -1752,8 +1998,11 @@
       <c r="H26" s="10">
         <v>31590</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>61</v>
       </c>
@@ -1778,8 +2027,11 @@
       <c r="H27" s="10">
         <v>29588</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="14" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>63</v>
       </c>
@@ -1804,8 +2056,11 @@
       <c r="H28" s="10">
         <v>30876</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="14" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>65</v>
       </c>
@@ -1830,8 +2085,11 @@
       <c r="H29" s="10">
         <v>29660</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="14" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>66</v>
       </c>
@@ -1856,8 +2114,11 @@
       <c r="H30" s="10">
         <v>33509</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="14" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>68</v>
       </c>
@@ -1882,8 +2143,11 @@
       <c r="H31" s="10">
         <v>29873</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="14" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>70</v>
       </c>
@@ -1908,8 +2172,11 @@
       <c r="H32" s="10">
         <v>31266</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="14" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>72</v>
       </c>
@@ -1934,8 +2201,11 @@
       <c r="H33" s="10">
         <v>32401</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>53</v>
       </c>
@@ -1960,8 +2230,11 @@
       <c r="H34" s="10">
         <v>36795</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="14" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>73</v>
       </c>
@@ -1986,8 +2259,11 @@
       <c r="H35" s="10">
         <v>30893</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>75</v>
       </c>
@@ -2012,8 +2288,11 @@
       <c r="H36" s="10">
         <v>34322</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="14" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>77</v>
       </c>
@@ -2038,8 +2317,11 @@
       <c r="H37" s="10">
         <v>31296</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>79</v>
       </c>
@@ -2064,8 +2346,11 @@
       <c r="H38" s="10">
         <v>30958</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>81</v>
       </c>
@@ -2090,8 +2375,11 @@
       <c r="H39" s="10">
         <v>34067</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="14" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>92</v>
       </c>
@@ -2116,8 +2404,11 @@
       <c r="H40" s="10">
         <v>33163</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="14" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>94</v>
       </c>
@@ -2142,8 +2433,11 @@
       <c r="H41" s="10">
         <v>32329</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="14" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>83</v>
       </c>
@@ -2168,8 +2462,11 @@
       <c r="H42" s="10">
         <v>32612</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="14" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>96</v>
       </c>
@@ -2194,8 +2491,11 @@
       <c r="H43" s="10">
         <v>32162</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>90</v>
       </c>
@@ -2220,8 +2520,11 @@
       <c r="H44" s="10">
         <v>30082</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="14" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>85</v>
       </c>
@@ -2246,8 +2549,11 @@
       <c r="H45" s="10">
         <v>31279</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="14" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>97</v>
       </c>
@@ -2272,8 +2578,11 @@
       <c r="H46" s="10">
         <v>35905</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="14" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>99</v>
       </c>
@@ -2298,8 +2607,11 @@
       <c r="H47" s="10">
         <v>31620</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>88</v>
       </c>
@@ -2324,8 +2636,11 @@
       <c r="H48" s="10">
         <v>31620</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="14" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>100</v>
       </c>
@@ -2350,8 +2665,11 @@
       <c r="H49" s="10">
         <v>30793</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="14" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>103</v>
       </c>
@@ -2376,8 +2694,11 @@
       <c r="H50" s="10">
         <v>30144</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="14" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>87</v>
       </c>
@@ -2402,8 +2723,11 @@
       <c r="H51" s="10">
         <v>36384</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="14" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -2413,7 +2737,7 @@
       <c r="G52" s="6"/>
       <c r="H52" s="7"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -2423,7 +2747,7 @@
       <c r="G53" s="6"/>
       <c r="H53" s="7"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H54" s="1"/>
     </row>
   </sheetData>

</xml_diff>